<commit_message>
Feat (Page Acceuil) : Button Dâte d'ajout & Recherche faite
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_MoreiraThomas.xlsx
+++ b/doc/Journal-de-Travail_MoreiraThomas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po51oro\Documents\GitHub\P_AppMobile-MoreiraThomas\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D15E418-7494-4777-BF5F-E17E47D32263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A084CF-B998-4F30-AC88-3DA3BFB99D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -134,6 +134,12 @@
   </si>
   <si>
     <t>Moreira Thomas</t>
+  </si>
+  <si>
+    <t>Finitions de la maquette</t>
+  </si>
+  <si>
+    <t>Commencer le Xaml de la page d'acceuil</t>
   </si>
 </sst>
 </file>
@@ -460,80 +466,6 @@
   <dxfs count="17">
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -701,6 +633,80 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1064,7 +1070,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>6.9444444444444448E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1079,7 +1085,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>9.7222222222222224E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1788,18 +1794,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="A6:G532" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="14">
+    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="6">
       <calculatedColumnFormula>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="heure" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Activité" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarque / problème" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="heure" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Activité" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarque / problème" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1995,7 +2001,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2048,7 +2054,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 2 heurs 30 minutes</v>
+        <v>0 jours 5 heurs 0 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2063,15 +2069,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2159,15 +2165,23 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="str">
+      <c r="A9" s="16">
         <f>IF(ISBLANK(B9),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B9))</f>
-        <v/>
-      </c>
-      <c r="B9" s="50"/>
+        <v>13</v>
+      </c>
+      <c r="B9" s="50">
+        <v>45744</v>
+      </c>
       <c r="C9" s="51"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="36"/>
+      <c r="D9" s="52">
+        <v>50</v>
+      </c>
+      <c r="E9" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>31</v>
+      </c>
       <c r="G9" s="56"/>
       <c r="M9" t="s">
         <v>4</v>
@@ -2180,15 +2194,25 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="str">
+      <c r="A10" s="8">
         <f>IF(ISBLANK(B10),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B10))</f>
-        <v/>
-      </c>
-      <c r="B10" s="46"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="36"/>
+        <v>13</v>
+      </c>
+      <c r="B10" s="46">
+        <v>45744</v>
+      </c>
+      <c r="C10" s="47">
+        <v>1</v>
+      </c>
+      <c r="D10" s="48">
+        <v>40</v>
+      </c>
+      <c r="E10" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>32</v>
+      </c>
       <c r="G10" s="55"/>
       <c r="M10" t="s">
         <v>5</v>
@@ -8528,28 +8552,28 @@
     <mergeCell ref="C5:D5"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:E532">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>$E7="Autre"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="2" stopIfTrue="1">
       <formula>$E7="Design"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="3" stopIfTrue="1">
       <formula>$E7="Présentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="4" stopIfTrue="1">
       <formula>$E7="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="5" stopIfTrue="1">
       <formula>$E7="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
       <formula>$E7="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="7" stopIfTrue="1">
       <formula>$E7="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>$E7="Développement"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8623,11 +8647,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8635,7 +8659,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0</v>
+        <v>6.9444444444444448E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8717,7 +8741,7 @@
       </c>
       <c r="B10">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C10,'Journal de travail'!$D$7:$D$532)</f>
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="C10" s="37" t="str">
         <f>'Journal de travail'!M14</f>
@@ -8725,7 +8749,7 @@
       </c>
       <c r="D10" s="33">
         <f t="shared" si="0"/>
-        <v>6.25E-2</v>
+        <v>9.7222222222222224E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -8752,7 +8776,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.10416666666666666</v>
+        <v>0.20833333333333331</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8775,6 +8799,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -8997,17 +9032,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9017,6 +9041,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9033,15 +9068,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat(Page d'acceuil) : toute la page est fini
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_MoreiraThomas.xlsx
+++ b/doc/Journal-de-Travail_MoreiraThomas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po51oro\Documents\GitHub\P_AppMobile-MoreiraThomas\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A084CF-B998-4F30-AC88-3DA3BFB99D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DF4051-7A66-47F0-AAB1-3895627FAA98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -140,6 +140,15 @@
   </si>
   <si>
     <t>Commencer le Xaml de la page d'acceuil</t>
+  </si>
+  <si>
+    <t>Disucussion de la classe avec le prog sur le projet</t>
+  </si>
+  <si>
+    <t>Finit le header</t>
+  </si>
+  <si>
+    <t>Body fini</t>
   </si>
 </sst>
 </file>
@@ -1070,7 +1079,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.9444444444444448E-2</c:v>
+                  <c:v>0.15277777777777779</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1088,7 +1097,7 @@
                   <c:v>9.7222222222222224E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1.0416666666666666E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2001,7 +2010,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2054,7 +2063,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 5 heurs 0 minutes</v>
+        <v>0 jours 7 heurs 15 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2069,15 +2078,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>120</v>
+        <v>195</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>300</v>
+        <v>435</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2225,15 +2234,23 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="str">
+      <c r="A11" s="16">
         <f>IF(ISBLANK(B11),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B11))</f>
-        <v/>
-      </c>
-      <c r="B11" s="50"/>
+        <v>14</v>
+      </c>
+      <c r="B11" s="50">
+        <v>45751</v>
+      </c>
       <c r="C11" s="51"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="36"/>
+      <c r="D11" s="52">
+        <v>15</v>
+      </c>
+      <c r="E11" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="36" t="s">
+        <v>33</v>
+      </c>
       <c r="G11" s="56"/>
       <c r="M11" t="s">
         <v>6</v>
@@ -2246,15 +2263,23 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="str">
+      <c r="A12" s="8">
         <f>IF(ISBLANK(B12),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B12))</f>
-        <v/>
-      </c>
-      <c r="B12" s="46"/>
+        <v>14</v>
+      </c>
+      <c r="B12" s="46">
+        <v>45751</v>
+      </c>
       <c r="C12" s="47"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="36"/>
+      <c r="D12" s="48">
+        <v>45</v>
+      </c>
+      <c r="E12" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>34</v>
+      </c>
       <c r="G12" s="55"/>
       <c r="M12" t="s">
         <v>7</v>
@@ -2267,15 +2292,25 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="str">
+      <c r="A13" s="16">
         <f>IF(ISBLANK(B13),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B13))</f>
-        <v/>
-      </c>
-      <c r="B13" s="50"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="36"/>
+        <v>14</v>
+      </c>
+      <c r="B13" s="50">
+        <v>45751</v>
+      </c>
+      <c r="C13" s="51">
+        <v>1</v>
+      </c>
+      <c r="D13" s="52">
+        <v>15</v>
+      </c>
+      <c r="E13" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>35</v>
+      </c>
       <c r="G13" s="56"/>
       <c r="M13" t="s">
         <v>8</v>
@@ -8647,11 +8682,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8659,7 +8694,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>6.9444444444444448E-2</v>
+        <v>0.15277777777777779</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8759,7 +8794,7 @@
       </c>
       <c r="B11">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C11,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C11" s="39" t="str">
         <f>'Journal de travail'!M15</f>
@@ -8767,7 +8802,7 @@
       </c>
       <c r="D11" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -8776,7 +8811,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.20833333333333331</v>
+        <v>0.30208333333333337</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8799,17 +8834,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9032,6 +9056,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9041,17 +9076,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9068,4 +9092,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat(Page du livre) : Page fait
[60][DONE]
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_MoreiraThomas.xlsx
+++ b/doc/Journal-de-Travail_MoreiraThomas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po51oro\Documents\GitHub\P_AppMobile-MoreiraThomas\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DF4051-7A66-47F0-AAB1-3895627FAA98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB9E92A-11FB-4CDC-8498-45EE101810D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>Body fini</t>
+  </si>
+  <si>
+    <t>Discussion pléniaire</t>
   </si>
 </sst>
 </file>
@@ -1097,7 +1100,7 @@
                   <c:v>9.7222222222222224E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0416666666666666E-2</c:v>
+                  <c:v>1.7361111111111112E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2010,7 +2013,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2063,7 +2066,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 7 heurs 15 minutes</v>
+        <v>0 jours 7 heurs 25 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2082,11 +2085,11 @@
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>435</v>
+        <v>445</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2323,15 +2326,23 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="str">
+      <c r="A14" s="8">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v/>
-      </c>
-      <c r="B14" s="46"/>
+        <v>15</v>
+      </c>
+      <c r="B14" s="46">
+        <v>45758</v>
+      </c>
       <c r="C14" s="47"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="36"/>
+      <c r="D14" s="48">
+        <v>10</v>
+      </c>
+      <c r="E14" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="36" t="s">
+        <v>36</v>
+      </c>
       <c r="G14" s="55"/>
       <c r="M14" t="s">
         <v>21</v>
@@ -2344,11 +2355,13 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="str">
+      <c r="A15" s="16">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B15))</f>
-        <v/>
-      </c>
-      <c r="B15" s="50"/>
+        <v>15</v>
+      </c>
+      <c r="B15" s="50">
+        <v>45758</v>
+      </c>
       <c r="C15" s="51"/>
       <c r="D15" s="52"/>
       <c r="E15" s="53"/>
@@ -8794,7 +8807,7 @@
       </c>
       <c r="B11">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C11,'Journal de travail'!$D$7:$D$532)</f>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C11" s="39" t="str">
         <f>'Journal de travail'!M15</f>
@@ -8802,7 +8815,7 @@
       </c>
       <c r="D11" s="33">
         <f t="shared" si="0"/>
-        <v>1.0416666666666666E-2</v>
+        <v>1.7361111111111112E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -8811,7 +8824,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.30208333333333337</v>
+        <v>0.30902777777777779</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8834,6 +8847,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9056,17 +9080,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9076,6 +9089,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9092,15 +9116,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat(Lecture) : Page de lecture fait
[30][DONE]
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_MoreiraThomas.xlsx
+++ b/doc/Journal-de-Travail_MoreiraThomas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po51oro\Documents\GitHub\P_AppMobile-MoreiraThomas\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB9E92A-11FB-4CDC-8498-45EE101810D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A25E58-CBF2-4B94-811A-CF3D2C2643E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -152,6 +152,21 @@
   </si>
   <si>
     <t>Discussion pléniaire</t>
+  </si>
+  <si>
+    <t>Chemin entre les pages faites</t>
+  </si>
+  <si>
+    <t>Page About fait</t>
+  </si>
+  <si>
+    <t>Page de lecture fait</t>
+  </si>
+  <si>
+    <t>Commencer la connection a la db</t>
+  </si>
+  <si>
+    <t>Release et preparer pour travailler chez soit</t>
   </si>
 </sst>
 </file>
@@ -1082,13 +1097,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.15277777777777779</c:v>
+                  <c:v>0.22916666666666666</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>3.472222222222222E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>4.1666666666666664E-2</c:v>
@@ -2013,7 +2028,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2066,7 +2081,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 7 heurs 25 minutes</v>
+        <v>0 jours 9 heurs 20 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2085,11 +2100,11 @@
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>205</v>
+        <v>320</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>445</v>
+        <v>560</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2363,9 +2378,15 @@
         <v>45758</v>
       </c>
       <c r="C15" s="51"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="36"/>
+      <c r="D15" s="52">
+        <v>40</v>
+      </c>
+      <c r="E15" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="36" t="s">
+        <v>37</v>
+      </c>
       <c r="G15" s="56"/>
       <c r="M15" t="s">
         <v>22</v>
@@ -2378,60 +2399,92 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="str">
+      <c r="A16" s="8">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B16))</f>
-        <v/>
-      </c>
-      <c r="B16" s="46"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="46">
+        <v>45758</v>
+      </c>
       <c r="C16" s="47"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="36"/>
+      <c r="D16" s="48">
+        <v>30</v>
+      </c>
+      <c r="E16" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="36" t="s">
+        <v>38</v>
+      </c>
       <c r="G16" s="55"/>
       <c r="O16">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="str">
+      <c r="A17" s="16">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
-        <v/>
-      </c>
-      <c r="B17" s="50"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="50">
+        <v>45758</v>
+      </c>
       <c r="C17" s="51"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="36"/>
+      <c r="D17" s="52">
+        <v>30</v>
+      </c>
+      <c r="E17" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="36" t="s">
+        <v>39</v>
+      </c>
       <c r="G17" s="56"/>
       <c r="O17">
         <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="str">
+      <c r="A18" s="8">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B18))</f>
-        <v/>
-      </c>
-      <c r="B18" s="46"/>
+        <v>15</v>
+      </c>
+      <c r="B18" s="46">
+        <v>45758</v>
+      </c>
       <c r="C18" s="47"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="36"/>
+      <c r="D18" s="48">
+        <v>10</v>
+      </c>
+      <c r="E18" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="36" t="s">
+        <v>40</v>
+      </c>
       <c r="G18" s="55"/>
       <c r="O18">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="str">
+      <c r="A19" s="16">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v/>
-      </c>
-      <c r="B19" s="50"/>
+        <v>15</v>
+      </c>
+      <c r="B19" s="50">
+        <v>45758</v>
+      </c>
       <c r="C19" s="51"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="36"/>
+      <c r="D19" s="52">
+        <v>5</v>
+      </c>
+      <c r="E19" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="36" t="s">
+        <v>41</v>
+      </c>
       <c r="G19" s="56"/>
       <c r="O19">
         <v>55</v>
@@ -8699,7 +8752,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>100</v>
+        <v>210</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8707,7 +8760,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.15277777777777779</v>
+        <v>0.22916666666666666</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8735,7 +8788,7 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C7" s="27" t="str">
         <f>'Journal de travail'!M11</f>
@@ -8743,7 +8796,7 @@
       </c>
       <c r="D7" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.472222222222222E-3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -8824,7 +8877,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.30902777777777779</v>
+        <v>0.38888888888888884</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8847,17 +8900,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9080,6 +9122,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9089,17 +9142,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9116,4 +9158,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
chore(DB) : DB connecter
[60][DONE]
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_MoreiraThomas.xlsx
+++ b/doc/Journal-de-Travail_MoreiraThomas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po51oro\Documents\GitHub\P_AppMobile-MoreiraThomas\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A25E58-CBF2-4B94-811A-CF3D2C2643E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF52E057-D716-420A-A374-537677D72637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -142,9 +142,6 @@
     <t>Commencer le Xaml de la page d'acceuil</t>
   </si>
   <si>
-    <t>Disucussion de la classe avec le prog sur le projet</t>
-  </si>
-  <si>
     <t>Finit le header</t>
   </si>
   <si>
@@ -167,6 +164,18 @@
   </si>
   <si>
     <t>Release et preparer pour travailler chez soit</t>
+  </si>
+  <si>
+    <t>Disucussion de la classe avec le prof sur le projet</t>
+  </si>
+  <si>
+    <t>Connections a la DB faite</t>
+  </si>
+  <si>
+    <t>Inserer les données de la DB</t>
+  </si>
+  <si>
+    <t>Crée et mis un logo pour l'app ainsi que divers petit ajustements</t>
   </si>
 </sst>
 </file>
@@ -1097,7 +1106,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.22916666666666666</c:v>
+                  <c:v>0.31944444444444442</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1115,7 +1124,7 @@
                   <c:v>9.7222222222222224E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.7361111111111112E-2</c:v>
+                  <c:v>2.7777777777777776E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2028,7 +2037,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2081,7 +2090,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 9 heurs 20 minutes</v>
+        <v>0 jours 11 heurs 45 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2096,15 +2105,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>240</v>
+        <v>300</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>320</v>
+        <v>405</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>560</v>
+        <v>705</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2267,7 +2276,7 @@
         <v>22</v>
       </c>
       <c r="F11" s="36" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="G11" s="56"/>
       <c r="M11" t="s">
@@ -2296,7 +2305,7 @@
         <v>4</v>
       </c>
       <c r="F12" s="36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G12" s="55"/>
       <c r="M12" t="s">
@@ -2327,7 +2336,7 @@
         <v>4</v>
       </c>
       <c r="F13" s="36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G13" s="56"/>
       <c r="M13" t="s">
@@ -2356,7 +2365,7 @@
         <v>22</v>
       </c>
       <c r="F14" s="36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G14" s="55"/>
       <c r="M14" t="s">
@@ -2385,7 +2394,7 @@
         <v>4</v>
       </c>
       <c r="F15" s="36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G15" s="56"/>
       <c r="M15" t="s">
@@ -2414,7 +2423,7 @@
         <v>4</v>
       </c>
       <c r="F16" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G16" s="55"/>
       <c r="O16">
@@ -2437,7 +2446,7 @@
         <v>4</v>
       </c>
       <c r="F17" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G17" s="56"/>
       <c r="O17">
@@ -2460,7 +2469,7 @@
         <v>4</v>
       </c>
       <c r="F18" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G18" s="55"/>
       <c r="O18">
@@ -2483,7 +2492,7 @@
         <v>6</v>
       </c>
       <c r="F19" s="36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G19" s="56"/>
       <c r="O19">
@@ -2491,51 +2500,85 @@
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="str">
+      <c r="A20" s="8">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B20))</f>
-        <v/>
-      </c>
-      <c r="B20" s="46"/>
+        <v>18</v>
+      </c>
+      <c r="B20" s="46">
+        <v>45779</v>
+      </c>
       <c r="C20" s="47"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="36"/>
+      <c r="D20" s="48">
+        <v>15</v>
+      </c>
+      <c r="E20" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="36" t="s">
+        <v>35</v>
+      </c>
       <c r="G20" s="55"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="str">
+      <c r="A21" s="16">
         <f>IF(ISBLANK(B21),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B21))</f>
-        <v/>
-      </c>
-      <c r="B21" s="50"/>
+        <v>18</v>
+      </c>
+      <c r="B21" s="50">
+        <v>45779</v>
+      </c>
       <c r="C21" s="51"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="36"/>
+      <c r="D21" s="52">
+        <v>40</v>
+      </c>
+      <c r="E21" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="36" t="s">
+        <v>42</v>
+      </c>
       <c r="G21" s="56"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="str">
+      <c r="A22" s="8">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
-        <v/>
-      </c>
-      <c r="B22" s="46"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="48"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="36"/>
+        <v>18</v>
+      </c>
+      <c r="B22" s="46">
+        <v>45779</v>
+      </c>
+      <c r="C22" s="47">
+        <v>1</v>
+      </c>
+      <c r="D22" s="48">
+        <v>0</v>
+      </c>
+      <c r="E22" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="36" t="s">
+        <v>43</v>
+      </c>
       <c r="G22" s="55"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="str">
+      <c r="A23" s="16">
         <f>IF(ISBLANK(B23),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B23))</f>
-        <v/>
-      </c>
-      <c r="B23" s="50"/>
+        <v>18</v>
+      </c>
+      <c r="B23" s="50">
+        <v>45779</v>
+      </c>
       <c r="C23" s="51"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="36"/>
+      <c r="D23" s="52">
+        <v>30</v>
+      </c>
+      <c r="E23" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="36" t="s">
+        <v>44</v>
+      </c>
       <c r="G23" s="56"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -8748,11 +8791,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>210</v>
+        <v>280</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8760,7 +8803,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.22916666666666666</v>
+        <v>0.31944444444444442</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8860,7 +8903,7 @@
       </c>
       <c r="B11">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C11,'Journal de travail'!$D$7:$D$532)</f>
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C11" s="39" t="str">
         <f>'Journal de travail'!M15</f>
@@ -8868,7 +8911,7 @@
       </c>
       <c r="D11" s="33">
         <f t="shared" si="0"/>
-        <v>1.7361111111111112E-2</v>
+        <v>2.7777777777777776E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -8877,7 +8920,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.38888888888888884</v>
+        <v>0.48958333333333331</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8900,6 +8943,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9122,17 +9176,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9142,6 +9185,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9158,15 +9212,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix(ALL) : fix des problemes pour les ViewModel
WIP
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_MoreiraThomas.xlsx
+++ b/doc/Journal-de-Travail_MoreiraThomas.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po51oro\Documents\GitHub\P_AppMobile-MoreiraThomas\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329F8774-2F66-4B68-BE2A-F489F9695E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D480330-85BC-4865-8E09-4E1FBC2EB5DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="5325" yWindow="1140" windowWidth="23400" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="48">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>Les données peuvent être utiliser mais il y a un probleme au ViewModel que j'ai pas eu le temps de modifier</t>
+  </si>
+  <si>
+    <t>Fix tout les problemes de touts les fichiers mais ça veut juste pas fonctionner les erreurs on aucune logiques</t>
   </si>
 </sst>
 </file>
@@ -1112,7 +1115,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.4861111111111111</c:v>
+                  <c:v>0.58680555555555558</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2096,7 +2099,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 16 heurs 25 minutes</v>
+        <v>0 jours 18 heurs 49 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2111,15 +2114,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>540</v>
+        <v>660</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>445</v>
+        <v>470</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>985</v>
+        <v>1130</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2672,15 +2675,25 @@
       <c r="G27" s="56"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="str">
+      <c r="A28" s="8">
         <f>IF(ISBLANK(B28),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B28))</f>
-        <v/>
-      </c>
-      <c r="B28" s="46"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="35"/>
+        <v>21</v>
+      </c>
+      <c r="B28" s="46">
+        <v>45800</v>
+      </c>
+      <c r="C28" s="47">
+        <v>2</v>
+      </c>
+      <c r="D28" s="48">
+        <v>25</v>
+      </c>
+      <c r="E28" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="35" t="s">
+        <v>47</v>
+      </c>
       <c r="G28" s="55"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -8833,11 +8846,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>420</v>
+        <v>540</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>280</v>
+        <v>305</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8845,7 +8858,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.4861111111111111</v>
+        <v>0.58680555555555558</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8962,7 +8975,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.68402777777777779</v>
+        <v>0.78472222222222221</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8985,17 +8998,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9218,6 +9220,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9227,17 +9240,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9254,4 +9256,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>